<commit_message>
Added coding of COND column
</commit_message>
<xml_diff>
--- a/data/oh/franklin/schema.xlsx
+++ b/data/oh/franklin/schema.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CTeuschler\Documents\Projects\ua-house-hunt\data\oh\franklin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8FF747-7C85-4600-801C-A676DC93DB9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A115ABC3-FEDC-44E2-95DC-22A3FB93AF20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5220" yWindow="4590" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schema" sheetId="1" r:id="rId1"/>
     <sheet name="Tax Only" sheetId="2" r:id="rId2"/>
     <sheet name="Both" sheetId="3" r:id="rId3"/>
+    <sheet name="Condition" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Tax Only'!$A$1:$E$77</definedName>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="174">
   <si>
     <t>'tax_only'</t>
   </si>
@@ -539,6 +540,24 @@
   </si>
   <si>
     <t>Contains NaN</t>
+  </si>
+  <si>
+    <t>POOR</t>
+  </si>
+  <si>
+    <t>FAIR</t>
+  </si>
+  <si>
+    <t>AVERAGE</t>
+  </si>
+  <si>
+    <t>GOOD</t>
+  </si>
+  <si>
+    <t>VERY GOOD</t>
+  </si>
+  <si>
+    <t>EXCELLENT</t>
   </si>
 </sst>
 </file>
@@ -2811,10 +2830,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2822,7 +2841,7 @@
     <col min="1" max="1" width="45.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>139</v>
       </c>
@@ -2835,48 +2854,32 @@
       <c r="E1" t="s">
         <v>162</v>
       </c>
-      <c r="I1" t="str">
-        <f>"df["&amp;A1&amp;"].unique()"</f>
-        <v>df[].unique()</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>100</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="I2" t="str">
-        <f t="shared" ref="I2:I40" si="0">"df["&amp;A2&amp;"].unique()"</f>
-        <v>df[ 'OBJECTID'].unique()</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>101</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="I3" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'PARCELID'].unique()</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>102</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="I4" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'LOWPARCELID'].unique()</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>103</v>
       </c>
@@ -2886,72 +2889,48 @@
       <c r="C5" t="s">
         <v>146</v>
       </c>
-      <c r="I5" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'STATEDAREA'].unique()</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>104</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="I6" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'ACRES'].unique()</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>105</v>
       </c>
       <c r="D7" t="s">
         <v>163</v>
       </c>
-      <c r="I7" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'CVTTXCD'].unique()</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>106</v>
       </c>
       <c r="D8" t="s">
         <v>165</v>
       </c>
-      <c r="I8" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'CVTTXDSCRP'].unique()</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>107</v>
       </c>
       <c r="D9" t="s">
         <v>165</v>
       </c>
-      <c r="I9" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'SCHLTXCD'].unique()</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>108</v>
       </c>
       <c r="D10" t="s">
         <v>165</v>
       </c>
-      <c r="I10" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'SCHLDSCRP'].unique()</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>109</v>
       </c>
@@ -2961,12 +2940,8 @@
       <c r="D11" t="s">
         <v>164</v>
       </c>
-      <c r="I11" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'NBHDTYP'].unique()</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>110</v>
       </c>
@@ -2979,12 +2954,8 @@
       <c r="D12" t="s">
         <v>164</v>
       </c>
-      <c r="I12" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'NBHDCD'].unique()</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>111</v>
       </c>
@@ -2994,12 +2965,8 @@
       <c r="D13" t="s">
         <v>164</v>
       </c>
-      <c r="I13" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'NBHDMODEL'].unique()</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>112</v>
       </c>
@@ -3009,12 +2976,8 @@
       <c r="D14" t="s">
         <v>166</v>
       </c>
-      <c r="I14" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'CLASSCD'].unique()</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>113</v>
       </c>
@@ -3024,126 +2987,74 @@
       <c r="D15" t="s">
         <v>166</v>
       </c>
-      <c r="I15" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'CLASSDSCRP'].unique()</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>114</v>
       </c>
-      <c r="I16" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'SITEADDRESS'].unique()</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>115</v>
       </c>
-      <c r="I17" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'ZIPCD'].unique()</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>116</v>
       </c>
-      <c r="I18" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'CNVYNAME'].unique()</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>117</v>
       </c>
-      <c r="I19" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'SALEDATE'].unique()</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>118</v>
       </c>
-      <c r="I20" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'RESFLRAREA_AG'].unique()</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>119</v>
       </c>
-      <c r="I21" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'RESFLRAREA_BG'].unique()</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>120</v>
       </c>
-      <c r="I22" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'RESFLRAREA'].unique()</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>121</v>
       </c>
-      <c r="I23" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'RESYRBLT'].unique()</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>122</v>
       </c>
-      <c r="I24" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'RESYRBLTEFF'].unique()</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>123</v>
       </c>
-      <c r="I25" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'RESSTRTYP'].unique()</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>124</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
-      <c r="I26" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'ROOMS'].unique()</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>125</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
-      <c r="I27" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'BATHS'].unique()</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>126</v>
       </c>
@@ -3153,12 +3064,8 @@
       <c r="D28" t="s">
         <v>167</v>
       </c>
-      <c r="I28" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'HBATHS'].unique()</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>127</v>
       </c>
@@ -3168,39 +3075,23 @@
       <c r="D29" t="s">
         <v>167</v>
       </c>
-      <c r="I29" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'BEDRMS'].unique()</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>128</v>
       </c>
-      <c r="I30" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'FIREPLC'].unique()</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>129</v>
       </c>
-      <c r="I31" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'AIRCOND'].unique()</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>130</v>
       </c>
-      <c r="I32" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'WALL'].unique()</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>131</v>
       </c>
@@ -3210,72 +3101,103 @@
       <c r="C33" t="s">
         <v>145</v>
       </c>
-      <c r="I33" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'COND'].unique()</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>132</v>
       </c>
-      <c r="I34" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'HEIGHT'].unique()</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>133</v>
       </c>
-      <c r="I35" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'BLDTYP'].unique()</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>134</v>
       </c>
-      <c r="I36" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'BLDGAREA'].unique()</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>135</v>
       </c>
-      <c r="I37" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'STRCLASS'].unique()</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>136</v>
       </c>
-      <c r="I38" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'X_COORD'].unique()</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>137</v>
       </c>
-      <c r="I39" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'Y_COORD'].unique()</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>138</v>
       </c>
-      <c r="I40" t="str">
-        <f t="shared" si="0"/>
-        <v>df[ 'LASTUPDATE'].unique()</v>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F3C938B-22BD-4C25-9409-169CD223A2EE}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>